<commit_message>
Remove a row inside the 'sensor_table_EXAMPLE.xlsx' that is just a comment but hinders the script to work properly
</commit_message>
<xml_diff>
--- a/sensor_table_EXAMPLE.xlsx
+++ b/sensor_table_EXAMPLE.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1014" uniqueCount="329">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1013" uniqueCount="328">
   <si>
     <t xml:space="preserve">uuid</t>
   </si>
@@ -923,9 +923,6 @@
   </si>
   <si>
     <t xml:space="preserve">Im Hydropulser fest verbaut</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Diverse Positionssensoren (TQ401) und Messumformer (IQS 450) im Lager Messtechnik vorhanden</t>
   </si>
   <si>
     <t xml:space="preserve">0184ebd9-988c-7bbb-9f6d-fca5fbdfdd0a</t>
@@ -1237,11 +1234,11 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="21" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="21" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1398,10 +1395,10 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="N1" activeCellId="0" sqref="N1"/>
       <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="A65" activeCellId="1" sqref="A11:V11 A65"/>
+      <selection pane="bottomRight" activeCell="A65" activeCellId="1" sqref="26:26 A65"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.4453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.4609375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="38.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.42"/>
@@ -5555,10 +5552,10 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="F34" activeCellId="1" sqref="A11:V11 F34"/>
+      <selection pane="bottomRight" activeCell="F34" activeCellId="1" sqref="26:26 F34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.4453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.4609375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="38.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.42"/>
@@ -6411,10 +6408,10 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="A11" activeCellId="0" sqref="A11:V11"/>
+      <selection pane="bottomRight" activeCell="A26" activeCellId="0" sqref="26:26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.4453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.4609375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="38.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.42"/>
@@ -7174,9 +7171,7 @@
       <c r="N25" s="8"/>
     </row>
     <row r="26" s="15" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B26" s="16" t="s">
-        <v>298</v>
-      </c>
+      <c r="B26" s="16"/>
       <c r="C26" s="16"/>
       <c r="D26" s="16"/>
       <c r="E26" s="16"/>
@@ -7285,10 +7280,10 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="I18" activeCellId="1" sqref="A11:V11 I18"/>
+      <selection pane="bottomRight" activeCell="I18" activeCellId="1" sqref="26:26 I18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.4453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.4609375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="38.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.42"/>
@@ -7401,10 +7396,10 @@
     </row>
     <row r="3" s="6" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="6" t="s">
+        <v>298</v>
+      </c>
+      <c r="B3" s="7" t="s">
         <v>299</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>300</v>
       </c>
       <c r="C3" s="6" t="n">
         <v>-50</v>
@@ -7413,7 +7408,7 @@
         <v>600</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="F3" s="6" t="n">
         <v>0</v>
@@ -7433,13 +7428,13 @@
         <v>-50</v>
       </c>
       <c r="K3" s="6" t="s">
+        <v>301</v>
+      </c>
+      <c r="L3" s="6" t="s">
         <v>302</v>
       </c>
-      <c r="L3" s="6" t="s">
+      <c r="N3" s="6" t="s">
         <v>303</v>
-      </c>
-      <c r="N3" s="6" t="s">
-        <v>304</v>
       </c>
       <c r="O3" s="7" t="n">
         <v>97450008</v>
@@ -7454,10 +7449,10 @@
     </row>
     <row r="4" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="6" t="s">
+        <v>304</v>
+      </c>
+      <c r="B4" s="7" t="s">
         <v>305</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>306</v>
       </c>
       <c r="C4" s="8" t="n">
         <v>-25</v>
@@ -7466,7 +7461,7 @@
         <v>100</v>
       </c>
       <c r="E4" s="17" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="F4" s="6" t="n">
         <v>0</v>
@@ -7486,16 +7481,16 @@
         <v>-25</v>
       </c>
       <c r="K4" s="8" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="L4" s="17" t="s">
+        <v>306</v>
+      </c>
+      <c r="N4" s="17" t="s">
         <v>307</v>
       </c>
-      <c r="N4" s="17" t="s">
+      <c r="O4" s="7" t="s">
         <v>308</v>
-      </c>
-      <c r="O4" s="7" t="s">
-        <v>309</v>
       </c>
       <c r="P4" s="17" t="s">
         <v>32</v>
@@ -7506,10 +7501,10 @@
     </row>
     <row r="5" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="6" t="s">
+        <v>309</v>
+      </c>
+      <c r="B5" s="7" t="s">
         <v>310</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>311</v>
       </c>
       <c r="C5" s="8" t="n">
         <v>-25</v>
@@ -7518,7 +7513,7 @@
         <v>150</v>
       </c>
       <c r="E5" s="17" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="F5" s="6" t="n">
         <v>0</v>
@@ -7538,13 +7533,13 @@
         <v>-25</v>
       </c>
       <c r="K5" s="8" t="s">
+        <v>311</v>
+      </c>
+      <c r="L5" s="17" t="s">
         <v>312</v>
       </c>
-      <c r="L5" s="17" t="s">
+      <c r="N5" s="17" t="s">
         <v>313</v>
-      </c>
-      <c r="N5" s="17" t="s">
-        <v>314</v>
       </c>
       <c r="O5" s="7" t="n">
         <v>163616</v>
@@ -7558,10 +7553,10 @@
     </row>
     <row r="6" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="6" t="s">
+        <v>314</v>
+      </c>
+      <c r="B6" s="7" t="s">
         <v>315</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>316</v>
       </c>
       <c r="C6" s="8" t="n">
         <v>0</v>
@@ -7570,7 +7565,7 @@
         <v>100</v>
       </c>
       <c r="E6" s="17" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="F6" s="6" t="n">
         <v>0</v>
@@ -7590,13 +7585,13 @@
         <v>0</v>
       </c>
       <c r="K6" s="8" t="s">
+        <v>311</v>
+      </c>
+      <c r="L6" s="17" t="s">
         <v>312</v>
       </c>
-      <c r="L6" s="17" t="s">
-        <v>313</v>
-      </c>
       <c r="N6" s="17" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="O6" s="7" t="n">
         <v>243008</v>
@@ -7612,10 +7607,10 @@
     </row>
     <row r="7" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="6" t="s">
+        <v>317</v>
+      </c>
+      <c r="B7" s="7" t="s">
         <v>318</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>319</v>
       </c>
       <c r="C7" s="8" t="n">
         <v>0</v>
@@ -7624,7 +7619,7 @@
         <v>100</v>
       </c>
       <c r="E7" s="17" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="F7" s="6" t="n">
         <v>0</v>
@@ -7644,13 +7639,13 @@
         <v>0</v>
       </c>
       <c r="K7" s="8" t="s">
+        <v>311</v>
+      </c>
+      <c r="L7" s="17" t="s">
         <v>312</v>
       </c>
-      <c r="L7" s="17" t="s">
-        <v>313</v>
-      </c>
       <c r="N7" s="6" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="O7" s="7" t="n">
         <v>203805</v>
@@ -7666,10 +7661,10 @@
     </row>
     <row r="8" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="6" t="s">
+        <v>319</v>
+      </c>
+      <c r="B8" s="7" t="s">
         <v>320</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>321</v>
       </c>
       <c r="C8" s="8" t="n">
         <v>-25</v>
@@ -7678,7 +7673,7 @@
         <v>100</v>
       </c>
       <c r="E8" s="17" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="F8" s="6" t="n">
         <v>0</v>
@@ -7698,16 +7693,16 @@
         <v>-25</v>
       </c>
       <c r="K8" s="8" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="L8" s="17" t="s">
+        <v>306</v>
+      </c>
+      <c r="N8" s="17" t="s">
         <v>307</v>
       </c>
-      <c r="N8" s="17" t="s">
-        <v>308</v>
-      </c>
       <c r="O8" s="7" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="P8" s="17" t="s">
         <v>32</v>
@@ -7720,10 +7715,10 @@
     </row>
     <row r="9" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="6" t="s">
+        <v>322</v>
+      </c>
+      <c r="B9" s="7" t="s">
         <v>323</v>
-      </c>
-      <c r="B9" s="7" t="s">
-        <v>324</v>
       </c>
       <c r="C9" s="6" t="n">
         <v>-40</v>
@@ -7732,7 +7727,7 @@
         <v>100</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="F9" s="6" t="n">
         <v>0</v>
@@ -7752,17 +7747,17 @@
         <v>-40</v>
       </c>
       <c r="K9" s="8" t="s">
+        <v>311</v>
+      </c>
+      <c r="L9" s="17" t="s">
         <v>312</v>
-      </c>
-      <c r="L9" s="17" t="s">
-        <v>313</v>
       </c>
       <c r="M9" s="8"/>
       <c r="N9" s="17" t="s">
+        <v>324</v>
+      </c>
+      <c r="O9" s="7" t="s">
         <v>325</v>
-      </c>
-      <c r="O9" s="7" t="s">
-        <v>326</v>
       </c>
       <c r="P9" s="17" t="s">
         <v>32</v>
@@ -7775,10 +7770,10 @@
     </row>
     <row r="10" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="6" t="s">
+        <v>326</v>
+      </c>
+      <c r="B10" s="7" t="s">
         <v>327</v>
-      </c>
-      <c r="B10" s="7" t="s">
-        <v>328</v>
       </c>
       <c r="C10" s="6" t="n">
         <v>-40</v>
@@ -7787,7 +7782,7 @@
         <v>100</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="F10" s="6" t="n">
         <v>0</v>
@@ -7807,17 +7802,17 @@
         <v>-40</v>
       </c>
       <c r="K10" s="8" t="s">
+        <v>311</v>
+      </c>
+      <c r="L10" s="17" t="s">
         <v>312</v>
-      </c>
-      <c r="L10" s="17" t="s">
-        <v>313</v>
       </c>
       <c r="M10" s="8"/>
       <c r="N10" s="17" t="s">
+        <v>324</v>
+      </c>
+      <c r="O10" s="7" t="s">
         <v>325</v>
-      </c>
-      <c r="O10" s="7" t="s">
-        <v>326</v>
       </c>
       <c r="P10" s="17" t="s">
         <v>32</v>

</xml_diff>

<commit_message>
Add a new example temperature sensor to the sensor_table_EXAMPLE.xlsx with uncertainties and the corresponding units
</commit_message>
<xml_diff>
--- a/sensor_table_EXAMPLE.xlsx
+++ b/sensor_table_EXAMPLE.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Druck" sheetId="1" state="visible" r:id="rId2"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1045" uniqueCount="336">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1057" uniqueCount="341">
   <si>
     <t xml:space="preserve">uuid</t>
   </si>
@@ -1041,6 +1041,21 @@
   </si>
   <si>
     <t xml:space="preserve">T23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">064f05d1-5d2d-7a6f-8000-a3da10f5a1a3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">T24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">°C/°C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pt1000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">648P016436</t>
   </si>
 </sst>
 </file>
@@ -1380,11 +1395,11 @@
   </sheetPr>
   <dimension ref="A1:AF203"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="AA3" activePane="bottomRight" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="2" ySplit="2" topLeftCell="AA21" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="AA1" activeCellId="0" sqref="AA1"/>
-      <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="bottomLeft" activeCell="A21" activeCellId="0" sqref="A21"/>
       <selection pane="bottomRight" activeCell="AF4" activeCellId="0" sqref="AF4"/>
     </sheetView>
   </sheetViews>
@@ -8115,12 +8130,12 @@
   </sheetPr>
   <dimension ref="A1:AD35"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="Y3" activePane="bottomRight" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="2" ySplit="2" topLeftCell="K3" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="Y1" activeCellId="0" sqref="Y1"/>
+      <selection pane="topRight" activeCell="K1" activeCellId="0" sqref="K1"/>
       <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomRight" activeCell="K11" activeCellId="0" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5078125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -8764,21 +8779,78 @@
       <c r="AD10" s="8"/>
     </row>
     <row r="11" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="7"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="8"/>
-      <c r="E11" s="17"/>
-      <c r="K11" s="8"/>
-      <c r="L11" s="17"/>
-      <c r="N11" s="17"/>
-      <c r="O11" s="19"/>
-      <c r="P11" s="17"/>
-      <c r="Q11" s="17"/>
-      <c r="R11" s="17"/>
-      <c r="S11" s="8"/>
-      <c r="T11" s="8"/>
+      <c r="A11" s="8" t="s">
+        <v>336</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>337</v>
+      </c>
+      <c r="C11" s="8" t="n">
+        <v>-25</v>
+      </c>
+      <c r="D11" s="8" t="n">
+        <v>100</v>
+      </c>
+      <c r="E11" s="17" t="s">
+        <v>308</v>
+      </c>
+      <c r="F11" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="G11" s="8" t="n">
+        <v>10</v>
+      </c>
+      <c r="H11" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="I11" s="8" t="n">
+        <f aca="false">(D11-C11)/(G11-F11)</f>
+        <v>12.5</v>
+      </c>
+      <c r="J11" s="8" t="n">
+        <f aca="false">D11-(I11*G11)</f>
+        <v>-25</v>
+      </c>
+      <c r="K11" s="0" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="L11" s="0" t="s">
+        <v>338</v>
+      </c>
+      <c r="M11" s="0"/>
+      <c r="N11" s="0"/>
+      <c r="O11" s="0" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="P11" s="0" t="s">
+        <v>308</v>
+      </c>
+      <c r="Q11" s="0"/>
+      <c r="R11" s="0"/>
+      <c r="S11" s="8" t="s">
+        <v>339</v>
+      </c>
+      <c r="T11" s="17" t="s">
+        <v>314</v>
+      </c>
       <c r="U11" s="8"/>
-      <c r="V11" s="8"/>
+      <c r="V11" s="17" t="s">
+        <v>315</v>
+      </c>
+      <c r="W11" s="7" t="s">
+        <v>340</v>
+      </c>
+      <c r="X11" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y11" s="8" t="s">
+        <v>197</v>
+      </c>
+      <c r="Z11" s="8"/>
+      <c r="AA11" s="8"/>
+      <c r="AB11" s="8"/>
+      <c r="AC11" s="8"/>
+      <c r="AD11" s="8"/>
     </row>
     <row r="12" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="7"/>

</xml_diff>

<commit_message>
Change the D096 pressure sensor bias from 0 ('absolut') to 1 ('relativ')
</commit_message>
<xml_diff>
--- a/sensor_table_EXAMPLE.xlsx
+++ b/sensor_table_EXAMPLE.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Druck" sheetId="1" state="visible" r:id="rId2"/>
@@ -15,13 +15,10 @@
   </sheets>
   <definedNames>
     <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Druck!$A$1:$AF$2</definedName>
-    <definedName function="false" hidden="true" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">Kraft!$A$1:$AD$2</definedName>
-    <definedName function="false" hidden="true" localSheetId="3" name="_xlnm._FilterDatabase" vbProcedure="false">Temperatur!$A$1:$AD$2</definedName>
-    <definedName function="false" hidden="true" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">Weg!$A$1:$AD$2</definedName>
+    <definedName function="false" hidden="true" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">Kraft!$A$1:$Z$2</definedName>
+    <definedName function="false" hidden="true" localSheetId="3" name="_xlnm._FilterDatabase" vbProcedure="false">Temperatur!$A$1:$Z$2</definedName>
+    <definedName function="false" hidden="true" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">Weg!$A$1:$Z$2</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Druck!$A$1:$AB$2</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">Kraft!$A$1:$Z$2</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">Weg!$A$1:$Z$2</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase" vbProcedure="false">Temperatur!$A$1:$Z$2</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -1309,6 +1306,37 @@
     <cellStyle name="Excel Built-in Neutral" xfId="21"/>
     <cellStyle name="Excel Built-in Note" xfId="22"/>
   </cellStyles>
+  <dxfs count="4">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF232629"/>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFAC090"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFCD5B5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -1395,15 +1423,15 @@
   </sheetPr>
   <dimension ref="A1:AF203"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="AA21" activePane="bottomRight" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="2" ySplit="2" topLeftCell="C36" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="AA1" activeCellId="0" sqref="AA1"/>
-      <selection pane="bottomLeft" activeCell="A21" activeCellId="0" sqref="A21"/>
-      <selection pane="bottomRight" activeCell="AF4" activeCellId="0" sqref="AF4"/>
+      <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A36" activeCellId="0" sqref="A36"/>
+      <selection pane="bottomRight" activeCell="F61" activeCellId="0" sqref="F61"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5078125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5234375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="38.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.42"/>
@@ -4986,7 +5014,7 @@
         <v>34</v>
       </c>
       <c r="F60" s="0" t="s">
-        <v>136</v>
+        <v>184</v>
       </c>
       <c r="G60" s="6" t="n">
         <v>0</v>
@@ -5002,8 +5030,7 @@
         <v>20</v>
       </c>
       <c r="K60" s="6" t="n">
-        <f aca="false">D60-(J60*H60)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L60" s="0"/>
       <c r="T60" s="8" t="s">
@@ -6143,8 +6170,8 @@
     <mergeCell ref="AF1:AF2"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.7875" bottom="0.7875" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.7875" bottom="0.7875" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -6168,7 +6195,7 @@
       <selection pane="bottomRight" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5078125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5234375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="38.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.42"/>
@@ -7094,7 +7121,7 @@
       <c r="B35" s="7"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AD2"/>
+  <autoFilter ref="A1:Z2"/>
   <mergeCells count="30">
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
@@ -7128,8 +7155,8 @@
     <mergeCell ref="AD1:AD2"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.7875" bottom="0.7875" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.7875" bottom="0.7875" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -7153,7 +7180,7 @@
       <selection pane="bottomRight" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5078125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5234375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="38.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.42"/>
@@ -8078,7 +8105,7 @@
       <c r="B35" s="7"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AD2"/>
+  <autoFilter ref="A1:Z2"/>
   <mergeCells count="31">
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
@@ -8113,8 +8140,8 @@
     <mergeCell ref="B26:M26"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.7875" bottom="0.7875" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.7875" bottom="0.7875" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -8130,7 +8157,7 @@
   </sheetPr>
   <dimension ref="A1:AD35"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="K3" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="K1" activeCellId="0" sqref="K1"/>
@@ -8138,7 +8165,7 @@
       <selection pane="bottomRight" activeCell="K11" activeCellId="0" sqref="K11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5078125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5234375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="38.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.42"/>
@@ -9128,7 +9155,7 @@
       <c r="M35" s="8"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AD2"/>
+  <autoFilter ref="A1:Z2"/>
   <mergeCells count="30">
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
@@ -9162,8 +9189,8 @@
     <mergeCell ref="AD1:AD2"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.7875" bottom="0.7875" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.7875" bottom="0.7875" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>

<commit_message>
Add the first uncertainty comments to the sensor_table_example.xlsx file
</commit_message>
<xml_diff>
--- a/sensor_table_EXAMPLE.xlsx
+++ b/sensor_table_EXAMPLE.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Druck" sheetId="1" state="visible" r:id="rId2"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1123" uniqueCount="356">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1210" uniqueCount="369">
   <si>
     <t xml:space="preserve">uuid</t>
   </si>
@@ -458,10 +458,16 @@
     <t xml:space="preserve">absolut</t>
   </si>
   <si>
+    <t xml:space="preserve">**Reference/relative** pressure sensor: 1 mbar or 0.05 %FS; **Absolute** pressure sensor: 0.5 mbar or 0.025 %FS (10…40 °C)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;= 0.1% FS </t>
+  </si>
+  <si>
     <t xml:space="preserve">PAA-33X/80794</t>
   </si>
   <si>
-    <t xml:space="preserve">S:\Rexer\02_Datenblaetter\datenblatt_150900_Keller_Drucksensor_33x+35x</t>
+    <t xml:space="preserve">S:\Rexer\02_Datenblaetter\datenblatt_150900_Keller_Drucksensor_33x+35x.pdf</t>
   </si>
   <si>
     <t xml:space="preserve">0184ebd9-988b-7bb9-bd33-2f48f7a868f2</t>
@@ -818,13 +824,25 @@
     <t xml:space="preserve">%/10K</t>
   </si>
   <si>
+    <t xml:space="preserve">???</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;= 1% FS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">müssten das hier nicht 0.04 %FS sein oder ist das Datenblatt falsch? &lt;= 0.05 %FS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt; 0.125% FS ??? bei 0.4Fnom?</t>
+  </si>
+  <si>
     <t xml:space="preserve">U10M/50kN</t>
   </si>
   <si>
     <t xml:space="preserve">014879S</t>
   </si>
   <si>
-    <t xml:space="preserve">S:\Rexer\02_Datenblaetter\datenblatt_000000_HBM_Kraftsensor_U10M</t>
+    <t xml:space="preserve">S:\Rexer\02_Datenblaetter\datenblatt_000000_HBM_Kraftsensor_U10M.pdf</t>
   </si>
   <si>
     <t xml:space="preserve">0184ebd9-988c-7bbb-9794-3dce416ae94d</t>
@@ -833,6 +851,12 @@
     <t xml:space="preserve">K08</t>
   </si>
   <si>
+    <t xml:space="preserve">&lt;= 0.04% FS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt; 0.1% FS</t>
+  </si>
+  <si>
     <t xml:space="preserve">U10M/25kN</t>
   </si>
   <si>
@@ -845,6 +869,12 @@
     <t xml:space="preserve">K09</t>
   </si>
   <si>
+    <t xml:space="preserve">&lt;= 0.03% FS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt; 0.075% FS</t>
+  </si>
+  <si>
     <t xml:space="preserve">U10M/5kN</t>
   </si>
   <si>
@@ -1013,7 +1043,10 @@
     <t xml:space="preserve">°C/°C</t>
   </si>
   <si>
-    <t xml:space="preserve">K</t>
+    <t xml:space="preserve">??? at room temperature (not defined) typical: &lt;= +-0.4% FS, maximal: &lt;= +-0.8% FS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UNKNOWN</t>
   </si>
   <si>
     <t xml:space="preserve">Pt1000</t>
@@ -1035,6 +1068,12 @@
   </si>
   <si>
     <t xml:space="preserve">T14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;= +-0.5°C (to the reference point)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt; 1% FS (depends on the single thermocouple)</t>
   </si>
   <si>
     <t xml:space="preserve">Messumformer/Thermoelement Typ K</t>
@@ -1109,7 +1148,7 @@
     <numFmt numFmtId="165" formatCode="0.00E+00"/>
     <numFmt numFmtId="166" formatCode="dd/mm/yyyy"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1146,6 +1185,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="7">
@@ -1258,7 +1303,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1280,6 +1325,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1312,6 +1361,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="22" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1448,12 +1501,12 @@
   </sheetPr>
   <dimension ref="A1:AK203"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="N3" activePane="bottomRight" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="2" ySplit="2" topLeftCell="K24" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="N1" activeCellId="0" sqref="N1"/>
-      <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="P13" activeCellId="0" sqref="P13"/>
+      <selection pane="topRight" activeCell="K1" activeCellId="0" sqref="K1"/>
+      <selection pane="bottomLeft" activeCell="A24" activeCellId="0" sqref="A24"/>
+      <selection pane="bottomRight" activeCell="AK45" activeCellId="0" sqref="AK45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1470,7 +1523,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="17.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="18.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="15" style="0" width="27"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="23.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="105.74"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="18" style="0" width="14.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="21.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="21" style="0" width="14.44"/>
@@ -3444,6 +3497,26 @@
         <f aca="false">D36-(J36*H36)</f>
         <v>0</v>
       </c>
+      <c r="O36" s="0" t="n">
+        <f aca="false"> (0.025/100)*(D36-C36)</f>
+        <v>0.00075</v>
+      </c>
+      <c r="P36" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q36" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="R36" s="0" t="n">
+        <f aca="false">(D36 - C36)*0.001</f>
+        <v>0.003</v>
+      </c>
+      <c r="S36" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="T36" s="6" t="s">
+        <v>143</v>
+      </c>
       <c r="X36" s="0" t="s">
         <v>41</v>
       </c>
@@ -3451,7 +3524,7 @@
         <v>42</v>
       </c>
       <c r="AA36" s="0" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="AB36" s="1" t="n">
         <v>148835</v>
@@ -3463,15 +3536,15 @@
         <v>50</v>
       </c>
       <c r="AK36" s="0" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="C37" s="0" t="n">
         <v>0</v>
@@ -3509,7 +3582,7 @@
         <v>42</v>
       </c>
       <c r="AA37" s="0" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="AB37" s="1" t="n">
         <v>5154</v>
@@ -3523,10 +3596,10 @@
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="C38" s="0" t="n">
         <v>0</v>
@@ -3578,10 +3651,10 @@
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="C39" s="0" t="n">
         <v>0</v>
@@ -3619,7 +3692,7 @@
         <v>42</v>
       </c>
       <c r="AA39" s="0" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="AB39" s="1" t="n">
         <v>74909</v>
@@ -3633,10 +3706,10 @@
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="C40" s="0" t="n">
         <v>0</v>
@@ -3674,7 +3747,7 @@
         <v>42</v>
       </c>
       <c r="AA40" s="0" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="AB40" s="1" t="n">
         <v>89574</v>
@@ -3688,10 +3761,10 @@
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="C41" s="0" t="n">
         <v>0</v>
@@ -3729,7 +3802,7 @@
         <v>42</v>
       </c>
       <c r="AA41" s="0" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="AB41" s="1" t="n">
         <v>74908</v>
@@ -3743,10 +3816,10 @@
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="C42" s="0" t="n">
         <v>0</v>
@@ -3784,7 +3857,7 @@
         <v>42</v>
       </c>
       <c r="AA42" s="0" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="AB42" s="1" t="n">
         <v>74907</v>
@@ -3798,10 +3871,10 @@
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="C43" s="0" t="n">
         <v>0</v>
@@ -3839,7 +3912,7 @@
         <v>42</v>
       </c>
       <c r="AA43" s="0" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="AB43" s="1" t="n">
         <v>88625</v>
@@ -3853,10 +3926,10 @@
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="C44" s="0" t="n">
         <v>0</v>
@@ -3894,7 +3967,7 @@
         <v>42</v>
       </c>
       <c r="AA44" s="0" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="AB44" s="1" t="n">
         <v>89576</v>
@@ -3908,10 +3981,10 @@
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="C45" s="0" t="n">
         <v>0</v>
@@ -3942,6 +4015,26 @@
         <f aca="false">D45-(J45*H45)</f>
         <v>0</v>
       </c>
+      <c r="O45" s="0" t="n">
+        <f aca="false"> (0.025/100)*(D45-C45)</f>
+        <v>0.0075</v>
+      </c>
+      <c r="P45" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q45" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="R45" s="0" t="n">
+        <f aca="false">(D45 - C45)*0.001</f>
+        <v>0.03</v>
+      </c>
+      <c r="S45" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="T45" s="6" t="s">
+        <v>143</v>
+      </c>
       <c r="X45" s="0" t="s">
         <v>41</v>
       </c>
@@ -3949,7 +4042,7 @@
         <v>42</v>
       </c>
       <c r="AA45" s="0" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="AB45" s="1" t="n">
         <v>428736</v>
@@ -3961,15 +4054,15 @@
         <v>50</v>
       </c>
       <c r="AK45" s="0" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="C46" s="0" t="n">
         <v>0</v>
@@ -4000,6 +4093,26 @@
         <f aca="false">D46-(J46*H46)</f>
         <v>0</v>
       </c>
+      <c r="O46" s="0" t="n">
+        <f aca="false"> (0.025/100)*(D46-C46)</f>
+        <v>0.0025</v>
+      </c>
+      <c r="P46" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q46" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="R46" s="0" t="n">
+        <f aca="false">(D46 - C46)*0.001</f>
+        <v>0.01</v>
+      </c>
+      <c r="S46" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="T46" s="6" t="s">
+        <v>143</v>
+      </c>
       <c r="X46" s="0" t="s">
         <v>41</v>
       </c>
@@ -4007,7 +4120,7 @@
         <v>42</v>
       </c>
       <c r="AA46" s="0" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="AB46" s="1" t="n">
         <v>605587</v>
@@ -4019,15 +4132,15 @@
         <v>50</v>
       </c>
       <c r="AK46" s="0" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="C47" s="0" t="n">
         <v>0</v>
@@ -4058,6 +4171,26 @@
         <f aca="false">D47-(J47*H47)</f>
         <v>0</v>
       </c>
+      <c r="O47" s="0" t="n">
+        <f aca="false"> (0.025/100)*(D47-C47)</f>
+        <v>0.0075</v>
+      </c>
+      <c r="P47" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q47" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="R47" s="0" t="n">
+        <f aca="false">(D47 - C47)*0.001</f>
+        <v>0.03</v>
+      </c>
+      <c r="S47" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="T47" s="6" t="s">
+        <v>143</v>
+      </c>
       <c r="X47" s="0" t="s">
         <v>41</v>
       </c>
@@ -4065,7 +4198,7 @@
         <v>42</v>
       </c>
       <c r="AA47" s="0" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="AB47" s="1" t="n">
         <v>353488</v>
@@ -4077,15 +4210,15 @@
         <v>50</v>
       </c>
       <c r="AK47" s="0" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="C48" s="0" t="n">
         <v>0</v>
@@ -4116,6 +4249,26 @@
         <f aca="false">D48-(J48*H48)</f>
         <v>0</v>
       </c>
+      <c r="O48" s="0" t="n">
+        <f aca="false"> (0.025/100)*(D48-C48)</f>
+        <v>0.075</v>
+      </c>
+      <c r="P48" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q48" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="R48" s="0" t="n">
+        <f aca="false">(D48 - C48)*0.001</f>
+        <v>0.3</v>
+      </c>
+      <c r="S48" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="T48" s="6" t="s">
+        <v>143</v>
+      </c>
       <c r="X48" s="0" t="s">
         <v>41</v>
       </c>
@@ -4123,7 +4276,7 @@
         <v>42</v>
       </c>
       <c r="AA48" s="0" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="AB48" s="1" t="n">
         <v>1090056</v>
@@ -4135,15 +4288,15 @@
         <v>50</v>
       </c>
       <c r="AK48" s="0" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="C49" s="0" t="n">
         <v>0</v>
@@ -4174,6 +4327,26 @@
         <f aca="false">D49-(J49*H49)</f>
         <v>0</v>
       </c>
+      <c r="O49" s="0" t="n">
+        <f aca="false"> (0.025/100)*(D49-C49)</f>
+        <v>0.075</v>
+      </c>
+      <c r="P49" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q49" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="R49" s="0" t="n">
+        <f aca="false">(D49 - C49)*0.001</f>
+        <v>0.3</v>
+      </c>
+      <c r="S49" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="T49" s="6" t="s">
+        <v>143</v>
+      </c>
       <c r="X49" s="0" t="s">
         <v>41</v>
       </c>
@@ -4181,7 +4354,7 @@
         <v>42</v>
       </c>
       <c r="AA49" s="0" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="AB49" s="1" t="n">
         <v>1090057</v>
@@ -4193,15 +4366,15 @@
         <v>50</v>
       </c>
       <c r="AK49" s="0" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="C50" s="0" t="n">
         <v>0</v>
@@ -4253,10 +4426,10 @@
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="C51" s="0" t="n">
         <v>0</v>
@@ -4294,7 +4467,7 @@
         <v>42</v>
       </c>
       <c r="AA51" s="0" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="AB51" s="1" t="n">
         <v>22588</v>
@@ -4308,10 +4481,10 @@
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="C52" s="0" t="n">
         <v>-10</v>
@@ -4343,13 +4516,13 @@
         <v>-10</v>
       </c>
       <c r="X52" s="1" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="Y52" s="0" t="s">
         <v>42</v>
       </c>
       <c r="AA52" s="0" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="AB52" s="1" t="n">
         <v>79699</v>
@@ -4363,10 +4536,10 @@
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="C53" s="0" t="n">
         <v>-20</v>
@@ -4398,13 +4571,13 @@
         <v>-20</v>
       </c>
       <c r="X53" s="1" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="Y53" s="0" t="s">
         <v>42</v>
       </c>
       <c r="AA53" s="0" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="AB53" s="1" t="n">
         <v>74999</v>
@@ -4418,10 +4591,10 @@
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="C54" s="0" t="n">
         <v>0</v>
@@ -4433,7 +4606,7 @@
         <v>39</v>
       </c>
       <c r="F54" s="0" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="G54" s="0" t="n">
         <v>0</v>
@@ -4456,10 +4629,10 @@
         <v>41</v>
       </c>
       <c r="Y54" s="0" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="AA54" s="0" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="AB54" s="1"/>
       <c r="AD54" s="0" t="s">
@@ -4471,10 +4644,10 @@
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="C55" s="0" t="n">
         <v>0</v>
@@ -4486,7 +4659,7 @@
         <v>39</v>
       </c>
       <c r="F55" s="0" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="G55" s="0" t="n">
         <v>0</v>
@@ -4509,10 +4682,10 @@
         <v>41</v>
       </c>
       <c r="Y55" s="0" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="AA55" s="0" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="AB55" s="1"/>
       <c r="AD55" s="0" t="s">
@@ -4524,10 +4697,10 @@
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="C56" s="0" t="n">
         <v>0</v>
@@ -4558,6 +4731,26 @@
         <f aca="false">D56-(J56*H56)</f>
         <v>0</v>
       </c>
+      <c r="O56" s="0" t="n">
+        <f aca="false"> (0.025/100)*(D56-C56)</f>
+        <v>0.0025</v>
+      </c>
+      <c r="P56" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q56" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="R56" s="0" t="n">
+        <f aca="false">(D56 - C56)*0.001</f>
+        <v>0.01</v>
+      </c>
+      <c r="S56" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="T56" s="6" t="s">
+        <v>143</v>
+      </c>
       <c r="X56" s="0" t="s">
         <v>41</v>
       </c>
@@ -4565,7 +4758,7 @@
         <v>42</v>
       </c>
       <c r="AA56" s="0" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="AB56" s="1" t="n">
         <v>1011246</v>
@@ -4577,15 +4770,15 @@
         <v>50</v>
       </c>
       <c r="AK56" s="0" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="C57" s="0" t="n">
         <v>0</v>
@@ -4616,6 +4809,26 @@
         <f aca="false">D57-(J57*H57)</f>
         <v>0</v>
       </c>
+      <c r="O57" s="0" t="n">
+        <f aca="false"> (0.025/100)*(D57-C57)</f>
+        <v>0.0025</v>
+      </c>
+      <c r="P57" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q57" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="R57" s="0" t="n">
+        <f aca="false">(D57 - C57)*0.001</f>
+        <v>0.01</v>
+      </c>
+      <c r="S57" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="T57" s="6" t="s">
+        <v>143</v>
+      </c>
       <c r="X57" s="0" t="s">
         <v>41</v>
       </c>
@@ -4623,7 +4836,7 @@
         <v>42</v>
       </c>
       <c r="AA57" s="0" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="AB57" s="1" t="n">
         <v>1011233</v>
@@ -4635,15 +4848,15 @@
         <v>50</v>
       </c>
       <c r="AK57" s="0" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="C58" s="0" t="n">
         <v>1</v>
@@ -4655,7 +4868,7 @@
         <v>39</v>
       </c>
       <c r="F58" s="0" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="G58" s="0" t="n">
         <v>0</v>
@@ -4681,7 +4894,7 @@
         <v>42</v>
       </c>
       <c r="AA58" s="0" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="AB58" s="1" t="n">
         <v>88662</v>
@@ -4690,15 +4903,15 @@
         <v>45</v>
       </c>
       <c r="AE58" s="0" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="C59" s="0" t="n">
         <v>1</v>
@@ -4710,7 +4923,7 @@
         <v>39</v>
       </c>
       <c r="F59" s="0" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="G59" s="0" t="n">
         <v>0</v>
@@ -4736,7 +4949,7 @@
         <v>42</v>
       </c>
       <c r="AA59" s="0" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="AB59" s="1" t="n">
         <v>25186</v>
@@ -4745,15 +4958,15 @@
         <v>45</v>
       </c>
       <c r="AE59" s="0" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="C60" s="0" t="n">
         <v>1</v>
@@ -4765,7 +4978,7 @@
         <v>39</v>
       </c>
       <c r="F60" s="0" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="G60" s="0" t="n">
         <v>0</v>
@@ -4790,7 +5003,7 @@
         <v>42</v>
       </c>
       <c r="AA60" s="0" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="AB60" s="1" t="n">
         <v>25185</v>
@@ -4799,15 +5012,15 @@
         <v>45</v>
       </c>
       <c r="AE60" s="0" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="C61" s="0" t="n">
         <v>0</v>
@@ -4845,22 +5058,22 @@
         <v>42</v>
       </c>
       <c r="AA61" s="0" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="AB61" s="1"/>
       <c r="AD61" s="0" t="s">
         <v>45</v>
       </c>
       <c r="AE61" s="0" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="C62" s="0" t="n">
         <v>0</v>
@@ -4891,6 +5104,26 @@
         <f aca="false">D62-(J62*H62)</f>
         <v>0</v>
       </c>
+      <c r="O62" s="0" t="n">
+        <f aca="false"> (0.025/100)*(D62-C62)</f>
+        <v>0.0125</v>
+      </c>
+      <c r="P62" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q62" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="R62" s="0" t="n">
+        <f aca="false">(D62 - C62)*0.001</f>
+        <v>0.05</v>
+      </c>
+      <c r="S62" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="T62" s="6" t="s">
+        <v>143</v>
+      </c>
       <c r="X62" s="0" t="s">
         <v>41</v>
       </c>
@@ -4898,7 +5131,7 @@
         <v>42</v>
       </c>
       <c r="AA62" s="0" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="AB62" s="1" t="n">
         <v>431003</v>
@@ -4907,18 +5140,18 @@
         <v>45</v>
       </c>
       <c r="AE62" s="0" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="AK62" s="0" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="C63" s="0" t="n">
         <v>0</v>
@@ -4950,18 +5183,25 @@
         <v>0</v>
       </c>
       <c r="O63" s="0" t="n">
-        <v>0.0005</v>
+        <f aca="false"> (0.025/100)*(D63-C63)</f>
+        <v>0.0125</v>
       </c>
       <c r="P63" s="0" t="s">
         <v>39</v>
       </c>
+      <c r="Q63" s="6" t="s">
+        <v>142</v>
+      </c>
       <c r="R63" s="0" t="n">
-        <f aca="false">(D63-C63)*0.001</f>
+        <f aca="false">(D63 - C63)*0.001</f>
         <v>0.05</v>
       </c>
       <c r="S63" s="0" t="s">
         <v>39</v>
       </c>
+      <c r="T63" s="6" t="s">
+        <v>143</v>
+      </c>
       <c r="X63" s="0" t="s">
         <v>41</v>
       </c>
@@ -4969,27 +5209,27 @@
         <v>42</v>
       </c>
       <c r="AA63" s="0" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="AB63" s="1" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="AD63" s="0" t="s">
         <v>45</v>
       </c>
       <c r="AE63" s="0" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="AK63" s="0" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="C64" s="0" t="n">
         <v>0</v>
@@ -5027,7 +5267,7 @@
         <v>42</v>
       </c>
       <c r="AA64" s="0" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="AB64" s="1" t="n">
         <v>126240</v>
@@ -5041,10 +5281,10 @@
     </row>
     <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="C65" s="0" t="n">
         <v>0</v>
@@ -5076,27 +5316,27 @@
       </c>
       <c r="X65" s="1"/>
       <c r="Y65" s="0" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="AA65" s="0" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="AB65" s="0" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="AD65" s="0" t="s">
         <v>45</v>
       </c>
       <c r="AJ65" s="0" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="C66" s="0" t="n">
         <v>0</v>
@@ -5108,7 +5348,7 @@
         <v>39</v>
       </c>
       <c r="F66" s="0" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="G66" s="0" t="n">
         <v>0</v>
@@ -5127,27 +5367,27 @@
       </c>
       <c r="X66" s="1"/>
       <c r="Y66" s="0" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="AA66" s="0" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="AB66" s="0" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="AD66" s="0" t="s">
         <v>45</v>
       </c>
       <c r="AJ66" s="0" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="C67" s="0" t="n">
         <v>0</v>
@@ -5179,27 +5419,27 @@
       </c>
       <c r="X67" s="1"/>
       <c r="Y67" s="0" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="AA67" s="0" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="AB67" s="0" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="AD67" s="0" t="s">
         <v>45</v>
       </c>
       <c r="AJ67" s="0" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="C68" s="0" t="n">
         <v>0</v>
@@ -5211,7 +5451,7 @@
         <v>39</v>
       </c>
       <c r="F68" s="0" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="G68" s="0" t="n">
         <v>0</v>
@@ -5230,19 +5470,19 @@
       </c>
       <c r="X68" s="1"/>
       <c r="Y68" s="0" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="AA68" s="0" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="AB68" s="0" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="AD68" s="0" t="s">
         <v>45</v>
       </c>
       <c r="AJ68" s="0" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5283,17 +5523,17 @@
     <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B76" s="1"/>
       <c r="O76" s="1"/>
-      <c r="S76" s="6"/>
+      <c r="S76" s="7"/>
     </row>
     <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B77" s="1"/>
       <c r="O77" s="1"/>
-      <c r="S77" s="6"/>
+      <c r="S77" s="7"/>
     </row>
     <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B78" s="1"/>
       <c r="O78" s="1"/>
-      <c r="S78" s="6"/>
+      <c r="S78" s="7"/>
     </row>
     <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B79" s="1"/>
@@ -5324,41 +5564,41 @@
       <c r="B88" s="1"/>
       <c r="O88" s="1"/>
       <c r="S88" s="1"/>
-      <c r="W88" s="7"/>
-      <c r="X88" s="7"/>
-      <c r="Y88" s="8"/>
+      <c r="W88" s="8"/>
+      <c r="X88" s="8"/>
+      <c r="Y88" s="9"/>
     </row>
     <row r="89" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B89" s="1"/>
       <c r="O89" s="1"/>
       <c r="S89" s="1"/>
-      <c r="W89" s="7"/>
-      <c r="X89" s="7"/>
-      <c r="Y89" s="8"/>
+      <c r="W89" s="8"/>
+      <c r="X89" s="8"/>
+      <c r="Y89" s="9"/>
     </row>
     <row r="90" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B90" s="1"/>
       <c r="O90" s="1"/>
       <c r="S90" s="1"/>
-      <c r="W90" s="7"/>
-      <c r="X90" s="7"/>
-      <c r="Y90" s="8"/>
+      <c r="W90" s="8"/>
+      <c r="X90" s="8"/>
+      <c r="Y90" s="9"/>
     </row>
     <row r="91" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B91" s="1"/>
       <c r="O91" s="1"/>
       <c r="S91" s="1"/>
-      <c r="W91" s="7"/>
-      <c r="X91" s="7"/>
-      <c r="Y91" s="8"/>
+      <c r="W91" s="8"/>
+      <c r="X91" s="8"/>
+      <c r="Y91" s="9"/>
     </row>
     <row r="92" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B92" s="1"/>
       <c r="O92" s="1"/>
       <c r="S92" s="1"/>
-      <c r="W92" s="7"/>
-      <c r="X92" s="7"/>
-      <c r="Y92" s="8"/>
+      <c r="W92" s="8"/>
+      <c r="X92" s="8"/>
+      <c r="Y92" s="9"/>
     </row>
     <row r="135" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="O135" s="1"/>
@@ -5626,12 +5866,12 @@
   </sheetPr>
   <dimension ref="A1:AI35"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="L3" activePane="bottomRight" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="2" ySplit="2" topLeftCell="I3" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="L1" activeCellId="0" sqref="L1"/>
+      <selection pane="topRight" activeCell="I1" activeCellId="0" sqref="I1"/>
       <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="AK4" activeCellId="0" sqref="AK4"/>
+      <selection pane="bottomRight" activeCell="M23" activeCellId="0" sqref="M23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5651,17 +5891,17 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="23.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="16" style="0" width="14.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="14.9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="22.48"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="30.76"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="14.9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="16.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="16.41"/>
   </cols>
   <sheetData>
     <row r="1" s="5" customFormat="true" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="9" t="s">
+      <c r="A1" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="10" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
@@ -5765,8 +6005,8 @@
       </c>
     </row>
     <row r="2" s="5" customFormat="true" ht="30.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="9"/>
-      <c r="B2" s="9"/>
+      <c r="A2" s="10"/>
+      <c r="B2" s="10"/>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
@@ -5803,10 +6043,10 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="C3" s="0" t="n">
         <v>0</v>
@@ -5815,7 +6055,7 @@
         <v>5</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="F3" s="0" t="n">
         <v>0</v>
@@ -5838,10 +6078,10 @@
         <v>113</v>
       </c>
       <c r="X3" s="0" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="Z3" s="0" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="AA3" s="1" t="n">
         <v>369955</v>
@@ -5855,10 +6095,10 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="C4" s="0" t="n">
         <v>0</v>
@@ -5867,7 +6107,7 @@
         <v>10</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="F4" s="0" t="n">
         <v>0</v>
@@ -5890,10 +6130,10 @@
         <v>113</v>
       </c>
       <c r="X4" s="0" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="Z4" s="0" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="AA4" s="1" t="n">
         <v>30893194</v>
@@ -5907,10 +6147,10 @@
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="C5" s="0" t="n">
         <v>0</v>
@@ -5919,7 +6159,7 @@
         <v>50</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="F5" s="0" t="n">
         <v>0</v>
@@ -5942,10 +6182,10 @@
         <v>113</v>
       </c>
       <c r="X5" s="0" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="Z5" s="0" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="AA5" s="1" t="n">
         <v>356069</v>
@@ -5959,10 +6199,10 @@
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="C6" s="0" t="n">
         <v>0</v>
@@ -5971,7 +6211,7 @@
         <v>10</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="F6" s="0" t="n">
         <v>0</v>
@@ -5994,13 +6234,13 @@
         <v>113</v>
       </c>
       <c r="X6" s="0" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="Z6" s="0" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="AA6" s="1" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="AB6" s="0" t="s">
         <v>45</v>
@@ -6011,10 +6251,10 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="C7" s="0" t="n">
         <v>0</v>
@@ -6023,7 +6263,7 @@
         <v>10</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="F7" s="0" t="n">
         <v>0</v>
@@ -6046,13 +6286,13 @@
         <v>113</v>
       </c>
       <c r="X7" s="0" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="Z7" s="0" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="AA7" s="1" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="AB7" s="0" t="s">
         <v>45</v>
@@ -6063,10 +6303,10 @@
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="C8" s="0" t="n">
         <v>0</v>
@@ -6075,7 +6315,7 @@
         <v>10</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="F8" s="0" t="n">
         <v>0</v>
@@ -6098,13 +6338,13 @@
         <v>113</v>
       </c>
       <c r="X8" s="0" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="Z8" s="0" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="AA8" s="1" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="AB8" s="0" t="s">
         <v>45</v>
@@ -6115,10 +6355,10 @@
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="C9" s="0" t="n">
         <v>0</v>
@@ -6127,7 +6367,7 @@
         <v>50</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="F9" s="0" t="n">
         <v>0</v>
@@ -6150,7 +6390,10 @@
         <v>0.00015</v>
       </c>
       <c r="L9" s="0" t="s">
-        <v>261</v>
+        <v>263</v>
+      </c>
+      <c r="M9" s="0" t="s">
+        <v>264</v>
       </c>
       <c r="N9" s="0" t="n">
         <f aca="false">(D9-C9)*0.01</f>
@@ -6160,6 +6403,9 @@
         <f aca="false">E9</f>
         <v>kN</v>
       </c>
+      <c r="P9" s="6" t="s">
+        <v>265</v>
+      </c>
       <c r="Q9" s="0" t="n">
         <f aca="false">(D9-C9)*0.0005</f>
         <v>0.025</v>
@@ -6168,6 +6414,9 @@
         <f aca="false">E9</f>
         <v>kN</v>
       </c>
+      <c r="S9" s="0" t="s">
+        <v>266</v>
+      </c>
       <c r="T9" s="0" t="n">
         <f aca="false">(D9-C9)*0.4*0.00125</f>
         <v>0.025</v>
@@ -6176,17 +6425,20 @@
         <f aca="false">E9</f>
         <v>kN</v>
       </c>
+      <c r="V9" s="0" t="s">
+        <v>267</v>
+      </c>
       <c r="W9" s="0" t="s">
         <v>113</v>
       </c>
       <c r="X9" s="0" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="Z9" s="0" t="s">
-        <v>262</v>
+        <v>268</v>
       </c>
       <c r="AA9" s="1" t="s">
-        <v>263</v>
+        <v>269</v>
       </c>
       <c r="AB9" s="0" t="s">
         <v>45</v>
@@ -6195,15 +6447,15 @@
         <v>50</v>
       </c>
       <c r="AI9" s="0" t="s">
-        <v>264</v>
+        <v>270</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>265</v>
+        <v>271</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>266</v>
+        <v>272</v>
       </c>
       <c r="C10" s="0" t="n">
         <v>0</v>
@@ -6212,7 +6464,7 @@
         <v>25</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="F10" s="0" t="n">
         <v>0</v>
@@ -6235,7 +6487,10 @@
         <v>0.00015</v>
       </c>
       <c r="L10" s="0" t="s">
-        <v>261</v>
+        <v>263</v>
+      </c>
+      <c r="M10" s="0" t="s">
+        <v>264</v>
       </c>
       <c r="N10" s="0" t="n">
         <f aca="false">(D10-C10)*0.01</f>
@@ -6245,6 +6500,9 @@
         <f aca="false">E10</f>
         <v>kN</v>
       </c>
+      <c r="P10" s="6" t="s">
+        <v>265</v>
+      </c>
       <c r="Q10" s="0" t="n">
         <f aca="false">(D10-C10)*0.0004</f>
         <v>0.01</v>
@@ -6253,6 +6511,9 @@
         <f aca="false">E10</f>
         <v>kN</v>
       </c>
+      <c r="S10" s="0" t="s">
+        <v>273</v>
+      </c>
       <c r="T10" s="0" t="n">
         <f aca="false">(D10-C10)*0.4*0.001</f>
         <v>0.01</v>
@@ -6261,17 +6522,20 @@
         <f aca="false">E10</f>
         <v>kN</v>
       </c>
+      <c r="V10" s="0" t="s">
+        <v>274</v>
+      </c>
       <c r="W10" s="0" t="s">
         <v>113</v>
       </c>
       <c r="X10" s="0" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="Z10" s="0" t="s">
-        <v>267</v>
+        <v>275</v>
       </c>
       <c r="AA10" s="1" t="s">
-        <v>268</v>
+        <v>276</v>
       </c>
       <c r="AB10" s="0" t="s">
         <v>45</v>
@@ -6280,15 +6544,15 @@
         <v>50</v>
       </c>
       <c r="AI10" s="0" t="s">
-        <v>264</v>
+        <v>270</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>269</v>
+        <v>277</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>270</v>
+        <v>278</v>
       </c>
       <c r="C11" s="0" t="n">
         <v>0</v>
@@ -6297,7 +6561,7 @@
         <v>5</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="F11" s="0" t="n">
         <v>0</v>
@@ -6320,7 +6584,10 @@
         <v>0.00015</v>
       </c>
       <c r="L11" s="0" t="s">
-        <v>261</v>
+        <v>263</v>
+      </c>
+      <c r="M11" s="0" t="s">
+        <v>264</v>
       </c>
       <c r="N11" s="0" t="n">
         <f aca="false">(D11-C11)*0.01</f>
@@ -6330,6 +6597,9 @@
         <f aca="false">E11</f>
         <v>kN</v>
       </c>
+      <c r="P11" s="6" t="s">
+        <v>265</v>
+      </c>
       <c r="Q11" s="0" t="n">
         <f aca="false">(D11-C11)*0.0003</f>
         <v>0.0015</v>
@@ -6338,6 +6608,9 @@
         <f aca="false">E11</f>
         <v>kN</v>
       </c>
+      <c r="S11" s="0" t="s">
+        <v>279</v>
+      </c>
       <c r="T11" s="0" t="n">
         <f aca="false">(D11-C11)*0.4*0.00075</f>
         <v>0.0015</v>
@@ -6346,17 +6619,20 @@
         <f aca="false">E11</f>
         <v>kN</v>
       </c>
+      <c r="V11" s="0" t="s">
+        <v>280</v>
+      </c>
       <c r="W11" s="0" t="s">
         <v>113</v>
       </c>
       <c r="X11" s="0" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="Z11" s="0" t="s">
-        <v>271</v>
+        <v>281</v>
       </c>
       <c r="AA11" s="1" t="s">
-        <v>272</v>
+        <v>282</v>
       </c>
       <c r="AB11" s="0" t="s">
         <v>45</v>
@@ -6365,15 +6641,15 @@
         <v>50</v>
       </c>
       <c r="AI11" s="0" t="s">
-        <v>264</v>
+        <v>270</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>273</v>
+        <v>283</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>274</v>
+        <v>284</v>
       </c>
       <c r="C12" s="0" t="n">
         <v>0</v>
@@ -6382,7 +6658,7 @@
         <v>50</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="F12" s="0" t="n">
         <v>0</v>
@@ -6405,10 +6681,10 @@
         <v>113</v>
       </c>
       <c r="X12" s="0" t="s">
-        <v>275</v>
+        <v>285</v>
       </c>
       <c r="Z12" s="0" t="s">
-        <v>276</v>
+        <v>286</v>
       </c>
       <c r="AA12" s="1" t="n">
         <v>50432</v>
@@ -6422,19 +6698,19 @@
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>277</v>
+        <v>287</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>278</v>
+        <v>288</v>
       </c>
       <c r="C13" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="D13" s="10" t="n">
+      <c r="D13" s="11" t="n">
         <v>12.5</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="F13" s="0" t="n">
         <v>0</v>
@@ -6457,7 +6733,10 @@
         <v>0.00015</v>
       </c>
       <c r="L13" s="0" t="s">
-        <v>261</v>
+        <v>263</v>
+      </c>
+      <c r="M13" s="0" t="s">
+        <v>264</v>
       </c>
       <c r="N13" s="0" t="n">
         <f aca="false">(D13-C13)*0.01</f>
@@ -6467,6 +6746,9 @@
         <f aca="false">E13</f>
         <v>kN</v>
       </c>
+      <c r="P13" s="6" t="s">
+        <v>265</v>
+      </c>
       <c r="Q13" s="0" t="n">
         <f aca="false">(D13-C13)*0.0004</f>
         <v>0.005</v>
@@ -6475,6 +6757,9 @@
         <f aca="false">E13</f>
         <v>kN</v>
       </c>
+      <c r="S13" s="0" t="s">
+        <v>273</v>
+      </c>
       <c r="T13" s="0" t="n">
         <f aca="false">(D13-C13)*0.4*0.001</f>
         <v>0.005</v>
@@ -6483,26 +6768,29 @@
         <f aca="false">E13</f>
         <v>kN</v>
       </c>
+      <c r="V13" s="0" t="s">
+        <v>274</v>
+      </c>
       <c r="W13" s="0" t="s">
         <v>113</v>
       </c>
       <c r="X13" s="0" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="Z13" s="0" t="s">
-        <v>279</v>
+        <v>289</v>
       </c>
       <c r="AA13" s="1" t="s">
-        <v>280</v>
+        <v>290</v>
       </c>
       <c r="AB13" s="0" t="s">
         <v>45</v>
       </c>
       <c r="AC13" s="0" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="AI13" s="0" t="s">
-        <v>264</v>
+        <v>270</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6634,12 +6922,12 @@
   </sheetPr>
   <dimension ref="A1:AI35"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="K3" activePane="bottomRight" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="2" ySplit="2" topLeftCell="M3" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="K1" activeCellId="0" sqref="K1"/>
+      <selection pane="topRight" activeCell="M1" activeCellId="0" sqref="M1"/>
       <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="AJ5" activeCellId="0" sqref="AJ5"/>
+      <selection pane="bottomRight" activeCell="R21" activeCellId="0" sqref="R21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6667,10 +6955,10 @@
   </cols>
   <sheetData>
     <row r="1" s="5" customFormat="true" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="9" t="s">
+      <c r="A1" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="10" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
@@ -6774,8 +7062,8 @@
       </c>
     </row>
     <row r="2" s="5" customFormat="true" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="9"/>
-      <c r="B2" s="9"/>
+      <c r="A2" s="10"/>
+      <c r="B2" s="10"/>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
@@ -6812,10 +7100,10 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>281</v>
+        <v>291</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>282</v>
+        <v>292</v>
       </c>
       <c r="C3" s="0" t="n">
         <v>0</v>
@@ -6824,7 +7112,7 @@
         <v>10</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>283</v>
+        <v>293</v>
       </c>
       <c r="F3" s="0" t="n">
         <v>0</v>
@@ -6844,13 +7132,13 @@
         <v>0</v>
       </c>
       <c r="W3" s="0" t="s">
-        <v>284</v>
+        <v>294</v>
       </c>
       <c r="X3" s="0" t="s">
-        <v>285</v>
+        <v>295</v>
       </c>
       <c r="Z3" s="0" t="s">
-        <v>286</v>
+        <v>296</v>
       </c>
       <c r="AA3" s="1" t="n">
         <v>826026</v>
@@ -6864,10 +7152,10 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>287</v>
+        <v>297</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>288</v>
+        <v>298</v>
       </c>
       <c r="C4" s="0" t="n">
         <v>0</v>
@@ -6876,7 +7164,7 @@
         <v>25</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>283</v>
+        <v>293</v>
       </c>
       <c r="F4" s="0" t="n">
         <v>0</v>
@@ -6896,13 +7184,13 @@
         <v>0</v>
       </c>
       <c r="W4" s="0" t="s">
-        <v>289</v>
+        <v>299</v>
       </c>
       <c r="X4" s="0" t="s">
-        <v>290</v>
+        <v>300</v>
       </c>
       <c r="Z4" s="0" t="s">
-        <v>291</v>
+        <v>301</v>
       </c>
       <c r="AA4" s="1" t="n">
         <v>130583</v>
@@ -6916,10 +7204,10 @@
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>292</v>
+        <v>302</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>293</v>
+        <v>303</v>
       </c>
       <c r="C5" s="0" t="n">
         <v>0</v>
@@ -6928,7 +7216,7 @@
         <v>25</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>283</v>
+        <v>293</v>
       </c>
       <c r="F5" s="0" t="n">
         <v>0</v>
@@ -6948,13 +7236,13 @@
         <v>0</v>
       </c>
       <c r="W5" s="0" t="s">
-        <v>289</v>
+        <v>299</v>
       </c>
       <c r="X5" s="0" t="s">
-        <v>290</v>
+        <v>300</v>
       </c>
       <c r="Z5" s="0" t="s">
-        <v>291</v>
+        <v>301</v>
       </c>
       <c r="AA5" s="1" t="n">
         <v>130584</v>
@@ -6968,10 +7256,10 @@
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>294</v>
+        <v>304</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>295</v>
+        <v>305</v>
       </c>
       <c r="C6" s="0" t="n">
         <v>0</v>
@@ -6980,7 +7268,7 @@
         <v>25</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>283</v>
+        <v>293</v>
       </c>
       <c r="F6" s="0" t="n">
         <v>0</v>
@@ -7000,13 +7288,13 @@
         <v>0</v>
       </c>
       <c r="W6" s="0" t="s">
-        <v>289</v>
+        <v>299</v>
       </c>
       <c r="X6" s="0" t="s">
-        <v>290</v>
+        <v>300</v>
       </c>
       <c r="Z6" s="0" t="s">
-        <v>291</v>
+        <v>301</v>
       </c>
       <c r="AA6" s="1" t="n">
         <v>130581</v>
@@ -7020,10 +7308,10 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>296</v>
+        <v>306</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>297</v>
+        <v>307</v>
       </c>
       <c r="C7" s="0" t="n">
         <v>65</v>
@@ -7032,7 +7320,7 @@
         <v>250</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>283</v>
+        <v>293</v>
       </c>
       <c r="F7" s="0" t="n">
         <v>0</v>
@@ -7052,13 +7340,13 @@
         <v>65</v>
       </c>
       <c r="W7" s="0" t="s">
-        <v>298</v>
+        <v>308</v>
       </c>
       <c r="X7" s="0" t="s">
-        <v>299</v>
+        <v>309</v>
       </c>
       <c r="Z7" s="0" t="s">
-        <v>300</v>
+        <v>310</v>
       </c>
       <c r="AA7" s="1" t="n">
         <v>25682</v>
@@ -7069,10 +7357,10 @@
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>301</v>
+        <v>311</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>302</v>
+        <v>312</v>
       </c>
       <c r="C8" s="0" t="n">
         <v>65</v>
@@ -7081,7 +7369,7 @@
         <v>250</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>283</v>
+        <v>293</v>
       </c>
       <c r="F8" s="0" t="n">
         <v>0</v>
@@ -7101,13 +7389,13 @@
         <v>65</v>
       </c>
       <c r="W8" s="0" t="s">
-        <v>298</v>
+        <v>308</v>
       </c>
       <c r="X8" s="0" t="s">
-        <v>299</v>
+        <v>309</v>
       </c>
       <c r="Z8" s="0" t="s">
-        <v>300</v>
+        <v>310</v>
       </c>
       <c r="AA8" s="1" t="n">
         <v>25662</v>
@@ -7118,10 +7406,10 @@
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>303</v>
+        <v>313</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>304</v>
+        <v>314</v>
       </c>
       <c r="C9" s="0" t="n">
         <v>0</v>
@@ -7130,7 +7418,7 @@
         <v>150</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>283</v>
+        <v>293</v>
       </c>
       <c r="F9" s="0" t="n">
         <v>0</v>
@@ -7150,13 +7438,13 @@
         <v>0</v>
       </c>
       <c r="W9" s="0" t="s">
-        <v>284</v>
+        <v>294</v>
       </c>
       <c r="X9" s="0" t="s">
-        <v>290</v>
+        <v>300</v>
       </c>
       <c r="Z9" s="0" t="s">
-        <v>305</v>
+        <v>315</v>
       </c>
       <c r="AA9" s="1"/>
       <c r="AB9" s="0" t="s">
@@ -7165,10 +7453,10 @@
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>306</v>
+        <v>316</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>307</v>
+        <v>317</v>
       </c>
       <c r="C10" s="0" t="n">
         <v>0</v>
@@ -7177,7 +7465,7 @@
         <v>225</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>283</v>
+        <v>293</v>
       </c>
       <c r="F10" s="0" t="n">
         <v>0</v>
@@ -7197,13 +7485,13 @@
         <v>0</v>
       </c>
       <c r="W10" s="0" t="s">
-        <v>284</v>
+        <v>294</v>
       </c>
       <c r="X10" s="0" t="s">
-        <v>290</v>
+        <v>300</v>
       </c>
       <c r="Z10" s="0" t="s">
-        <v>308</v>
+        <v>318</v>
       </c>
       <c r="AA10" s="1"/>
       <c r="AB10" s="0" t="s">
@@ -7212,10 +7500,10 @@
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>309</v>
+        <v>319</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>310</v>
+        <v>320</v>
       </c>
       <c r="C11" s="0" t="n">
         <v>0</v>
@@ -7224,7 +7512,7 @@
         <v>300</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>283</v>
+        <v>293</v>
       </c>
       <c r="F11" s="0" t="n">
         <v>-10</v>
@@ -7245,31 +7533,34 @@
         <v>0.005</v>
       </c>
       <c r="R11" s="0" t="s">
-        <v>311</v>
+        <v>321</v>
+      </c>
+      <c r="S11" s="0" t="s">
+        <v>264</v>
       </c>
       <c r="W11" s="1" t="s">
-        <v>312</v>
+        <v>322</v>
       </c>
       <c r="X11" s="0" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="Z11" s="0" t="s">
-        <v>313</v>
+        <v>323</v>
       </c>
       <c r="AA11" s="0" t="s">
-        <v>314</v>
+        <v>324</v>
       </c>
       <c r="AB11" s="0" t="s">
         <v>45</v>
       </c>
       <c r="AC11" s="0" t="s">
-        <v>315</v>
+        <v>325</v>
       </c>
       <c r="AH11" s="0" t="s">
-        <v>316</v>
+        <v>326</v>
       </c>
       <c r="AI11" s="0" t="s">
-        <v>317</v>
+        <v>327</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7308,19 +7599,19 @@
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="1"/>
     </row>
-    <row r="26" s="11" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B26" s="12"/>
-      <c r="C26" s="12"/>
-      <c r="D26" s="12"/>
-      <c r="E26" s="12"/>
-      <c r="F26" s="12"/>
-      <c r="G26" s="12"/>
-      <c r="H26" s="12"/>
-      <c r="I26" s="12"/>
-      <c r="J26" s="12"/>
-      <c r="K26" s="12"/>
-      <c r="L26" s="12"/>
-      <c r="M26" s="12"/>
+    <row r="26" s="12" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B26" s="13"/>
+      <c r="C26" s="13"/>
+      <c r="D26" s="13"/>
+      <c r="E26" s="13"/>
+      <c r="F26" s="13"/>
+      <c r="G26" s="13"/>
+      <c r="H26" s="13"/>
+      <c r="I26" s="13"/>
+      <c r="J26" s="13"/>
+      <c r="K26" s="13"/>
+      <c r="L26" s="13"/>
+      <c r="M26" s="13"/>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="1"/>
@@ -7407,12 +7698,12 @@
   </sheetPr>
   <dimension ref="A1:AI35"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="2" ySplit="2" topLeftCell="N3" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
+      <selection pane="topRight" activeCell="N1" activeCellId="0" sqref="N1"/>
       <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="M11" activeCellId="0" sqref="M11"/>
+      <selection pane="bottomRight" activeCell="S17" activeCellId="0" sqref="S17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -7428,23 +7719,23 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="9" style="0" width="23.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="17.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="15.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="26.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="65.08"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="21.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="23.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="23.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="28.95"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="14.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="13.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="23.77"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="42.23"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="17.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="18.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="19.14"/>
   </cols>
   <sheetData>
     <row r="1" s="5" customFormat="true" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="9" t="s">
+      <c r="A1" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="10" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
@@ -7548,8 +7839,8 @@
       </c>
     </row>
     <row r="2" s="5" customFormat="true" ht="30.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="9"/>
-      <c r="B2" s="9"/>
+      <c r="A2" s="10"/>
+      <c r="B2" s="10"/>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
@@ -7586,10 +7877,10 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>318</v>
+        <v>328</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>319</v>
+        <v>329</v>
       </c>
       <c r="C3" s="0" t="n">
         <v>-50</v>
@@ -7598,7 +7889,7 @@
         <v>600</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>320</v>
+        <v>330</v>
       </c>
       <c r="F3" s="0" t="n">
         <v>0</v>
@@ -7618,13 +7909,13 @@
         <v>-50</v>
       </c>
       <c r="W3" s="0" t="s">
-        <v>321</v>
+        <v>331</v>
       </c>
       <c r="X3" s="0" t="s">
-        <v>322</v>
+        <v>332</v>
       </c>
       <c r="Z3" s="0" t="s">
-        <v>323</v>
+        <v>333</v>
       </c>
       <c r="AA3" s="1" t="n">
         <v>97450008</v>
@@ -7638,10 +7929,10 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>324</v>
+        <v>334</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>325</v>
+        <v>335</v>
       </c>
       <c r="C4" s="0" t="n">
         <v>-25</v>
@@ -7649,8 +7940,8 @@
       <c r="D4" s="0" t="n">
         <v>100</v>
       </c>
-      <c r="E4" s="13" t="s">
-        <v>320</v>
+      <c r="E4" s="14" t="s">
+        <v>330</v>
       </c>
       <c r="F4" s="0" t="n">
         <v>0</v>
@@ -7673,45 +7964,54 @@
         <v>0.5</v>
       </c>
       <c r="L4" s="0" t="s">
-        <v>326</v>
+        <v>336</v>
+      </c>
+      <c r="M4" s="0" t="s">
+        <v>337</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>338</v>
       </c>
       <c r="Q4" s="0" t="n">
         <v>0.5</v>
       </c>
       <c r="R4" s="0" t="s">
-        <v>327</v>
-      </c>
-      <c r="T4" s="0" t="n">
-        <v>0</v>
+        <v>330</v>
+      </c>
+      <c r="S4" s="15" t="s">
+        <v>264</v>
+      </c>
+      <c r="T4" s="1" t="s">
+        <v>338</v>
       </c>
       <c r="W4" s="0" t="s">
-        <v>328</v>
-      </c>
-      <c r="X4" s="13" t="s">
-        <v>329</v>
-      </c>
-      <c r="Z4" s="13" t="s">
-        <v>330</v>
+        <v>339</v>
+      </c>
+      <c r="X4" s="14" t="s">
+        <v>340</v>
+      </c>
+      <c r="Z4" s="14" t="s">
+        <v>341</v>
       </c>
       <c r="AA4" s="1" t="s">
-        <v>331</v>
-      </c>
-      <c r="AB4" s="13" t="s">
+        <v>342</v>
+      </c>
+      <c r="AB4" s="14" t="s">
         <v>45</v>
       </c>
       <c r="AC4" s="0" t="s">
         <v>50</v>
       </c>
       <c r="AI4" s="0" t="s">
-        <v>332</v>
+        <v>343</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>333</v>
+        <v>344</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>334</v>
+        <v>345</v>
       </c>
       <c r="C5" s="0" t="n">
         <v>-25</v>
@@ -7719,8 +8019,8 @@
       <c r="D5" s="0" t="n">
         <v>150</v>
       </c>
-      <c r="E5" s="13" t="s">
-        <v>320</v>
+      <c r="E5" s="14" t="s">
+        <v>330</v>
       </c>
       <c r="F5" s="0" t="n">
         <v>0</v>
@@ -7739,53 +8039,59 @@
         <f aca="false">D5-(I5*G5)</f>
         <v>-25</v>
       </c>
-      <c r="K5" s="1" t="n">
-        <v>0</v>
+      <c r="K5" s="1" t="s">
+        <v>338</v>
       </c>
       <c r="N5" s="0" t="n">
         <v>0.5</v>
       </c>
       <c r="O5" s="0" t="s">
-        <v>320</v>
+        <v>330</v>
+      </c>
+      <c r="P5" s="0" t="s">
+        <v>346</v>
       </c>
       <c r="Q5" s="0" t="n">
         <f aca="false">(D5-C5)*0.01</f>
         <v>1.75</v>
       </c>
       <c r="R5" s="0" t="s">
-        <v>327</v>
-      </c>
-      <c r="T5" s="0" t="n">
-        <v>0</v>
+        <v>330</v>
+      </c>
+      <c r="S5" s="0" t="s">
+        <v>347</v>
+      </c>
+      <c r="T5" s="1" t="s">
+        <v>338</v>
       </c>
       <c r="W5" s="0" t="s">
-        <v>335</v>
-      </c>
-      <c r="X5" s="13" t="s">
-        <v>336</v>
-      </c>
-      <c r="Z5" s="13" t="s">
-        <v>337</v>
+        <v>348</v>
+      </c>
+      <c r="X5" s="14" t="s">
+        <v>349</v>
+      </c>
+      <c r="Z5" s="14" t="s">
+        <v>350</v>
       </c>
       <c r="AA5" s="1" t="n">
         <v>163616</v>
       </c>
-      <c r="AB5" s="13" t="s">
+      <c r="AB5" s="14" t="s">
         <v>45</v>
       </c>
       <c r="AC5" s="0" t="s">
         <v>50</v>
       </c>
       <c r="AI5" s="0" t="s">
-        <v>338</v>
+        <v>351</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>339</v>
+        <v>352</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>340</v>
+        <v>353</v>
       </c>
       <c r="C6" s="0" t="n">
         <v>0</v>
@@ -7793,8 +8099,8 @@
       <c r="D6" s="0" t="n">
         <v>100</v>
       </c>
-      <c r="E6" s="13" t="s">
-        <v>320</v>
+      <c r="E6" s="14" t="s">
+        <v>330</v>
       </c>
       <c r="F6" s="0" t="n">
         <v>0</v>
@@ -7813,54 +8119,60 @@
         <f aca="false">D6-(I6*G6)</f>
         <v>0</v>
       </c>
-      <c r="K6" s="1" t="n">
-        <v>0</v>
+      <c r="K6" s="1" t="s">
+        <v>338</v>
       </c>
       <c r="N6" s="0" t="n">
         <v>0.5</v>
       </c>
       <c r="O6" s="0" t="s">
-        <v>320</v>
+        <v>330</v>
+      </c>
+      <c r="P6" s="0" t="s">
+        <v>346</v>
       </c>
       <c r="Q6" s="0" t="n">
         <f aca="false">(D6-C6)*0.01</f>
         <v>1</v>
       </c>
       <c r="R6" s="0" t="s">
-        <v>327</v>
-      </c>
-      <c r="T6" s="0" t="n">
-        <v>0</v>
+        <v>330</v>
+      </c>
+      <c r="S6" s="0" t="s">
+        <v>347</v>
+      </c>
+      <c r="T6" s="1" t="s">
+        <v>338</v>
       </c>
       <c r="W6" s="0" t="s">
-        <v>335</v>
-      </c>
-      <c r="X6" s="13" t="s">
-        <v>336</v>
-      </c>
-      <c r="Z6" s="13" t="s">
-        <v>341</v>
+        <v>348</v>
+      </c>
+      <c r="X6" s="14" t="s">
+        <v>349</v>
+      </c>
+      <c r="Z6" s="14" t="s">
+        <v>354</v>
       </c>
       <c r="AA6" s="1" t="n">
         <v>243008</v>
       </c>
-      <c r="AB6" s="13" t="s">
+      <c r="AB6" s="14" t="s">
         <v>45</v>
       </c>
       <c r="AC6" s="0" t="s">
         <v>50</v>
       </c>
-      <c r="AF6" s="8"/>
+      <c r="AF6" s="9"/>
       <c r="AI6" s="0" t="s">
-        <v>338</v>
+        <v>351</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>342</v>
+        <v>355</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>343</v>
+        <v>356</v>
       </c>
       <c r="C7" s="0" t="n">
         <v>0</v>
@@ -7868,8 +8180,8 @@
       <c r="D7" s="0" t="n">
         <v>100</v>
       </c>
-      <c r="E7" s="13" t="s">
-        <v>320</v>
+      <c r="E7" s="14" t="s">
+        <v>330</v>
       </c>
       <c r="F7" s="0" t="n">
         <v>0</v>
@@ -7888,54 +8200,60 @@
         <f aca="false">D7-(I7*G7)</f>
         <v>0</v>
       </c>
-      <c r="K7" s="1" t="n">
-        <v>0</v>
+      <c r="K7" s="1" t="s">
+        <v>338</v>
       </c>
       <c r="N7" s="0" t="n">
         <v>0.5</v>
       </c>
       <c r="O7" s="0" t="s">
-        <v>320</v>
+        <v>330</v>
+      </c>
+      <c r="P7" s="0" t="s">
+        <v>346</v>
       </c>
       <c r="Q7" s="0" t="n">
         <f aca="false">(D7-C7)*0.01</f>
         <v>1</v>
       </c>
       <c r="R7" s="0" t="s">
-        <v>327</v>
-      </c>
-      <c r="T7" s="0" t="n">
-        <v>0</v>
+        <v>330</v>
+      </c>
+      <c r="S7" s="0" t="s">
+        <v>347</v>
+      </c>
+      <c r="T7" s="1" t="s">
+        <v>338</v>
       </c>
       <c r="W7" s="0" t="s">
-        <v>335</v>
-      </c>
-      <c r="X7" s="13" t="s">
-        <v>336</v>
+        <v>348</v>
+      </c>
+      <c r="X7" s="14" t="s">
+        <v>349</v>
       </c>
       <c r="Z7" s="0" t="s">
-        <v>341</v>
+        <v>354</v>
       </c>
       <c r="AA7" s="1" t="n">
         <v>203805</v>
       </c>
-      <c r="AB7" s="13" t="s">
+      <c r="AB7" s="14" t="s">
         <v>45</v>
       </c>
       <c r="AC7" s="0" t="s">
         <v>50</v>
       </c>
-      <c r="AF7" s="8"/>
+      <c r="AF7" s="9"/>
       <c r="AI7" s="0" t="s">
-        <v>338</v>
+        <v>351</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>344</v>
+        <v>357</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>345</v>
+        <v>358</v>
       </c>
       <c r="C8" s="0" t="n">
         <v>-25</v>
@@ -7943,8 +8261,8 @@
       <c r="D8" s="0" t="n">
         <v>100</v>
       </c>
-      <c r="E8" s="13" t="s">
-        <v>320</v>
+      <c r="E8" s="14" t="s">
+        <v>330</v>
       </c>
       <c r="F8" s="0" t="n">
         <v>0</v>
@@ -7967,46 +8285,55 @@
         <v>0.5</v>
       </c>
       <c r="L8" s="0" t="s">
-        <v>326</v>
+        <v>336</v>
+      </c>
+      <c r="M8" s="0" t="s">
+        <v>264</v>
+      </c>
+      <c r="N8" s="1" t="s">
+        <v>338</v>
       </c>
       <c r="Q8" s="0" t="n">
         <v>0.5</v>
       </c>
       <c r="R8" s="0" t="s">
-        <v>327</v>
-      </c>
-      <c r="T8" s="0" t="n">
-        <v>0</v>
+        <v>330</v>
+      </c>
+      <c r="S8" s="15" t="s">
+        <v>264</v>
+      </c>
+      <c r="T8" s="1" t="s">
+        <v>338</v>
       </c>
       <c r="W8" s="0" t="s">
-        <v>328</v>
-      </c>
-      <c r="X8" s="13" t="s">
-        <v>329</v>
-      </c>
-      <c r="Z8" s="13" t="s">
-        <v>330</v>
+        <v>339</v>
+      </c>
+      <c r="X8" s="14" t="s">
+        <v>340</v>
+      </c>
+      <c r="Z8" s="14" t="s">
+        <v>341</v>
       </c>
       <c r="AA8" s="1" t="s">
-        <v>346</v>
-      </c>
-      <c r="AB8" s="13" t="s">
+        <v>359</v>
+      </c>
+      <c r="AB8" s="14" t="s">
         <v>45</v>
       </c>
       <c r="AC8" s="0" t="s">
-        <v>203</v>
-      </c>
-      <c r="AF8" s="8"/>
+        <v>205</v>
+      </c>
+      <c r="AF8" s="9"/>
       <c r="AI8" s="0" t="s">
-        <v>332</v>
+        <v>343</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>347</v>
+        <v>360</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>348</v>
+        <v>361</v>
       </c>
       <c r="C9" s="0" t="n">
         <v>-40</v>
@@ -8015,7 +8342,7 @@
         <v>100</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>320</v>
+        <v>330</v>
       </c>
       <c r="F9" s="0" t="n">
         <v>0</v>
@@ -8034,54 +8361,60 @@
         <f aca="false">D9-(I9*G9)</f>
         <v>-40</v>
       </c>
-      <c r="K9" s="1" t="n">
-        <v>0</v>
+      <c r="K9" s="1" t="s">
+        <v>338</v>
       </c>
       <c r="N9" s="0" t="n">
         <v>0.5</v>
       </c>
       <c r="O9" s="0" t="s">
-        <v>320</v>
+        <v>330</v>
+      </c>
+      <c r="P9" s="0" t="s">
+        <v>346</v>
       </c>
       <c r="Q9" s="0" t="n">
         <f aca="false">(D9-C9)*0.01</f>
         <v>1.4</v>
       </c>
       <c r="R9" s="0" t="s">
-        <v>327</v>
-      </c>
-      <c r="T9" s="0" t="n">
-        <v>0</v>
+        <v>330</v>
+      </c>
+      <c r="S9" s="0" t="s">
+        <v>347</v>
+      </c>
+      <c r="T9" s="1" t="s">
+        <v>338</v>
       </c>
       <c r="W9" s="0" t="s">
-        <v>335</v>
-      </c>
-      <c r="X9" s="13" t="s">
-        <v>336</v>
-      </c>
-      <c r="Z9" s="13" t="s">
+        <v>348</v>
+      </c>
+      <c r="X9" s="14" t="s">
         <v>349</v>
       </c>
+      <c r="Z9" s="14" t="s">
+        <v>362</v>
+      </c>
       <c r="AA9" s="1" t="s">
-        <v>350</v>
-      </c>
-      <c r="AB9" s="13" t="s">
+        <v>363</v>
+      </c>
+      <c r="AB9" s="14" t="s">
         <v>45</v>
       </c>
       <c r="AC9" s="0" t="s">
         <v>50</v>
       </c>
-      <c r="AF9" s="8"/>
+      <c r="AF9" s="9"/>
       <c r="AI9" s="0" t="s">
-        <v>338</v>
+        <v>351</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>351</v>
+        <v>364</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>352</v>
+        <v>365</v>
       </c>
       <c r="C10" s="0" t="n">
         <v>-40</v>
@@ -8090,7 +8423,7 @@
         <v>100</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>320</v>
+        <v>330</v>
       </c>
       <c r="F10" s="0" t="n">
         <v>0</v>
@@ -8109,54 +8442,60 @@
         <f aca="false">D10-(I10*G10)</f>
         <v>-40</v>
       </c>
-      <c r="K10" s="1" t="n">
-        <v>0</v>
+      <c r="K10" s="1" t="s">
+        <v>338</v>
       </c>
       <c r="N10" s="0" t="n">
         <v>0.5</v>
       </c>
       <c r="O10" s="0" t="s">
-        <v>320</v>
+        <v>330</v>
+      </c>
+      <c r="P10" s="0" t="s">
+        <v>346</v>
       </c>
       <c r="Q10" s="0" t="n">
         <f aca="false">(D10-C10)*0.01</f>
         <v>1.4</v>
       </c>
       <c r="R10" s="0" t="s">
-        <v>327</v>
-      </c>
-      <c r="T10" s="0" t="n">
-        <v>0</v>
+        <v>330</v>
+      </c>
+      <c r="S10" s="0" t="s">
+        <v>347</v>
+      </c>
+      <c r="T10" s="1" t="s">
+        <v>338</v>
       </c>
       <c r="W10" s="0" t="s">
-        <v>335</v>
-      </c>
-      <c r="X10" s="13" t="s">
-        <v>336</v>
-      </c>
-      <c r="Z10" s="13" t="s">
+        <v>348</v>
+      </c>
+      <c r="X10" s="14" t="s">
         <v>349</v>
       </c>
+      <c r="Z10" s="14" t="s">
+        <v>362</v>
+      </c>
       <c r="AA10" s="1" t="s">
-        <v>350</v>
-      </c>
-      <c r="AB10" s="13" t="s">
+        <v>363</v>
+      </c>
+      <c r="AB10" s="14" t="s">
         <v>45</v>
       </c>
       <c r="AC10" s="0" t="s">
         <v>50</v>
       </c>
-      <c r="AD10" s="13"/>
+      <c r="AD10" s="14"/>
       <c r="AI10" s="0" t="s">
-        <v>338</v>
+        <v>351</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>353</v>
+        <v>366</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>354</v>
+        <v>367</v>
       </c>
       <c r="C11" s="0" t="n">
         <v>-25</v>
@@ -8164,8 +8503,8 @@
       <c r="D11" s="0" t="n">
         <v>100</v>
       </c>
-      <c r="E11" s="13" t="s">
-        <v>320</v>
+      <c r="E11" s="14" t="s">
+        <v>330</v>
       </c>
       <c r="F11" s="0" t="n">
         <v>0</v>
@@ -8188,90 +8527,99 @@
         <v>0.5</v>
       </c>
       <c r="L11" s="0" t="s">
-        <v>326</v>
+        <v>336</v>
+      </c>
+      <c r="M11" s="0" t="s">
+        <v>264</v>
+      </c>
+      <c r="N11" s="1" t="s">
+        <v>338</v>
       </c>
       <c r="Q11" s="0" t="n">
         <v>0.5</v>
       </c>
       <c r="R11" s="0" t="s">
-        <v>327</v>
-      </c>
-      <c r="T11" s="0" t="n">
-        <v>0</v>
+        <v>330</v>
+      </c>
+      <c r="S11" s="15" t="s">
+        <v>264</v>
+      </c>
+      <c r="T11" s="1" t="s">
+        <v>338</v>
       </c>
       <c r="W11" s="0" t="s">
-        <v>328</v>
-      </c>
-      <c r="X11" s="13" t="s">
-        <v>329</v>
-      </c>
-      <c r="Z11" s="13" t="s">
-        <v>330</v>
+        <v>339</v>
+      </c>
+      <c r="X11" s="14" t="s">
+        <v>340</v>
+      </c>
+      <c r="Z11" s="14" t="s">
+        <v>341</v>
       </c>
       <c r="AA11" s="1" t="s">
-        <v>355</v>
-      </c>
-      <c r="AB11" s="13" t="s">
+        <v>368</v>
+      </c>
+      <c r="AB11" s="14" t="s">
         <v>45</v>
       </c>
       <c r="AC11" s="0" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="AI11" s="0" t="s">
-        <v>332</v>
+        <v>343</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="1"/>
-      <c r="E12" s="13"/>
-      <c r="L12" s="13"/>
-      <c r="N12" s="13"/>
-      <c r="O12" s="14"/>
-      <c r="P12" s="13"/>
-      <c r="Q12" s="13"/>
-      <c r="R12" s="13"/>
-    </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E12" s="14"/>
+      <c r="L12" s="14"/>
+      <c r="N12" s="14"/>
+      <c r="O12" s="16"/>
+      <c r="P12" s="14"/>
+      <c r="Q12" s="14"/>
+      <c r="R12" s="14"/>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="1"/>
-      <c r="E13" s="13"/>
-      <c r="L13" s="13"/>
-      <c r="N13" s="13"/>
-      <c r="O13" s="14"/>
-      <c r="P13" s="13"/>
-      <c r="Q13" s="13"/>
-      <c r="R13" s="13"/>
+      <c r="E13" s="14"/>
+      <c r="L13" s="14"/>
+      <c r="N13" s="14"/>
+      <c r="O13" s="16"/>
+      <c r="P13" s="14"/>
+      <c r="Q13" s="14"/>
+      <c r="R13" s="14"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="1"/>
-      <c r="E14" s="13"/>
-      <c r="L14" s="13"/>
-      <c r="N14" s="13"/>
+      <c r="E14" s="14"/>
+      <c r="L14" s="14"/>
+      <c r="N14" s="14"/>
       <c r="O14" s="1"/>
-      <c r="P14" s="13"/>
-      <c r="Q14" s="13"/>
+      <c r="P14" s="14"/>
+      <c r="Q14" s="14"/>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="1"/>
-      <c r="L20" s="13"/>
-      <c r="N20" s="13"/>
+      <c r="L20" s="14"/>
+      <c r="N20" s="14"/>
       <c r="O20" s="1"/>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="1"/>
-      <c r="L21" s="13"/>
-      <c r="N21" s="13"/>
+      <c r="L21" s="14"/>
+      <c r="N21" s="14"/>
       <c r="O21" s="1"/>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="1"/>
-      <c r="L22" s="13"/>
-      <c r="N22" s="13"/>
+      <c r="L22" s="14"/>
+      <c r="N22" s="14"/>
       <c r="O22" s="1"/>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="1"/>
-      <c r="L23" s="13"/>
-      <c r="N23" s="13"/>
+      <c r="L23" s="14"/>
+      <c r="N23" s="14"/>
       <c r="O23" s="1"/>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>